<commit_message>
macro and meso but meso useless too much info
</commit_message>
<xml_diff>
--- a/data/intermediate/reseau/recategorize_designation.xlsx
+++ b/data/intermediate/reseau/recategorize_designation.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://genes-my.sharepoint.com/personal/lmaurice_ensae_fr/Documents/CCNE/Analyse/CCNE/data/intermediate/reseau/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="601" documentId="11_B89231273C696DEBE4B4ADE2E75D06D0725D8531" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{0C1E7115-698B-4DCB-8D9F-E8C6F14B0EAE}"/>
+  <xr:revisionPtr revIDLastSave="610" documentId="11_B89231273C696DEBE4B4ADE2E75D06D0725D8531" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{5D20DBC1-B9B3-473A-834A-FC92FFA503E9}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15720" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="667" uniqueCount="266">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="667" uniqueCount="265">
   <si>
     <t>Désignation</t>
   </si>
@@ -718,9 +718,6 @@
     <t>Religion</t>
   </si>
   <si>
-    <t>Organisations internationales</t>
-  </si>
-  <si>
     <t>AFSS</t>
   </si>
   <si>
@@ -787,9 +784,6 @@
     <t>Philosophes antiques</t>
   </si>
   <si>
-    <t>Science et littérature</t>
-  </si>
-  <si>
     <t>Autobiographie</t>
   </si>
   <si>
@@ -802,15 +796,9 @@
     <t>Fondations caritatives</t>
   </si>
   <si>
-    <t>Expertise, Forums, Autorités</t>
-  </si>
-  <si>
     <t>Traités divers</t>
   </si>
   <si>
-    <t>Loi diverses</t>
-  </si>
-  <si>
     <t>Ministères Education, Recherche, Enseignement</t>
   </si>
   <si>
@@ -818,6 +806,15 @@
   </si>
   <si>
     <t>Agence française de sécurité sanitaire de l’environnement et du travail</t>
+  </si>
+  <si>
+    <t>Science, littérature</t>
+  </si>
+  <si>
+    <t>Forums, Autorités</t>
+  </si>
+  <si>
+    <t>Org Internationales</t>
   </si>
 </sst>
 </file>
@@ -870,10 +867,6 @@
     </ext>
   </extLst>
 </styleSheet>
-</file>
-
-<file path=xl/persons/person.xml><?xml version="1.0" encoding="utf-8"?>
-<personList xmlns="http://schemas.microsoft.com/office/spreadsheetml/2018/threadedcomments" xmlns:x="http://schemas.openxmlformats.org/spreadsheetml/2006/main"/>
 </file>
 
 <file path=xl/tables/table1.xml><?xml version="1.0" encoding="utf-8"?>
@@ -1173,8 +1166,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:D222"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A72" workbookViewId="0">
-      <selection activeCell="H83" sqref="H83"/>
+    <sheetView tabSelected="1" topLeftCell="A35" workbookViewId="0">
+      <selection activeCell="I50" sqref="I50"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1206,10 +1199,10 @@
         <v>266</v>
       </c>
       <c r="C2" t="s">
-        <v>248</v>
+        <v>247</v>
       </c>
       <c r="D2" t="s">
-        <v>255</v>
+        <v>262</v>
       </c>
     </row>
     <row r="3" spans="1:4" x14ac:dyDescent="0.25">
@@ -1223,7 +1216,7 @@
         <v>173</v>
       </c>
       <c r="D3" t="s">
-        <v>255</v>
+        <v>262</v>
       </c>
     </row>
     <row r="4" spans="1:4" x14ac:dyDescent="0.25">
@@ -1237,7 +1230,7 @@
         <v>209</v>
       </c>
       <c r="D4" t="s">
-        <v>255</v>
+        <v>262</v>
       </c>
     </row>
     <row r="5" spans="1:4" x14ac:dyDescent="0.25">
@@ -1248,10 +1241,10 @@
         <v>83</v>
       </c>
       <c r="C5" t="s">
-        <v>245</v>
+        <v>244</v>
       </c>
       <c r="D5" t="s">
-        <v>255</v>
+        <v>262</v>
       </c>
     </row>
     <row r="6" spans="1:4" x14ac:dyDescent="0.25">
@@ -1276,10 +1269,10 @@
         <v>39</v>
       </c>
       <c r="C7" t="s">
-        <v>242</v>
+        <v>241</v>
       </c>
       <c r="D7" t="s">
-        <v>255</v>
+        <v>262</v>
       </c>
     </row>
     <row r="8" spans="1:4" x14ac:dyDescent="0.25">
@@ -1290,7 +1283,7 @@
         <v>32</v>
       </c>
       <c r="C8" t="s">
-        <v>241</v>
+        <v>240</v>
       </c>
       <c r="D8" t="s">
         <v>228</v>
@@ -1304,10 +1297,10 @@
         <v>31</v>
       </c>
       <c r="C9" t="s">
-        <v>245</v>
+        <v>244</v>
       </c>
       <c r="D9" t="s">
-        <v>255</v>
+        <v>262</v>
       </c>
     </row>
     <row r="10" spans="1:4" x14ac:dyDescent="0.25">
@@ -1388,10 +1381,10 @@
         <v>23</v>
       </c>
       <c r="C15" t="s">
-        <v>252</v>
+        <v>251</v>
       </c>
       <c r="D15" t="s">
-        <v>255</v>
+        <v>262</v>
       </c>
     </row>
     <row r="16" spans="1:4" x14ac:dyDescent="0.25">
@@ -1402,10 +1395,10 @@
         <v>23</v>
       </c>
       <c r="C16" t="s">
-        <v>244</v>
+        <v>243</v>
       </c>
       <c r="D16" t="s">
-        <v>255</v>
+        <v>262</v>
       </c>
     </row>
     <row r="17" spans="1:4" x14ac:dyDescent="0.25">
@@ -1419,7 +1412,7 @@
         <v>154</v>
       </c>
       <c r="D17" t="s">
-        <v>232</v>
+        <v>264</v>
       </c>
     </row>
     <row r="18" spans="1:4" x14ac:dyDescent="0.25">
@@ -1472,10 +1465,10 @@
         <v>20</v>
       </c>
       <c r="C21" t="s">
-        <v>243</v>
+        <v>242</v>
       </c>
       <c r="D21" t="s">
-        <v>255</v>
+        <v>262</v>
       </c>
     </row>
     <row r="22" spans="1:4" x14ac:dyDescent="0.25">
@@ -1486,10 +1479,10 @@
         <v>20</v>
       </c>
       <c r="C22" t="s">
-        <v>248</v>
+        <v>247</v>
       </c>
       <c r="D22" t="s">
-        <v>255</v>
+        <v>262</v>
       </c>
     </row>
     <row r="23" spans="1:4" x14ac:dyDescent="0.25">
@@ -1517,7 +1510,7 @@
         <v>155</v>
       </c>
       <c r="D24" t="s">
-        <v>232</v>
+        <v>264</v>
       </c>
     </row>
     <row r="25" spans="1:4" x14ac:dyDescent="0.25">
@@ -1528,7 +1521,7 @@
         <v>19</v>
       </c>
       <c r="C25" t="s">
-        <v>246</v>
+        <v>245</v>
       </c>
       <c r="D25" t="s">
         <v>221</v>
@@ -1570,10 +1563,10 @@
         <v>17</v>
       </c>
       <c r="C28" t="s">
-        <v>242</v>
+        <v>241</v>
       </c>
       <c r="D28" t="s">
-        <v>255</v>
+        <v>262</v>
       </c>
     </row>
     <row r="29" spans="1:4" x14ac:dyDescent="0.25">
@@ -1601,7 +1594,7 @@
         <v>9</v>
       </c>
       <c r="D30" t="s">
-        <v>260</v>
+        <v>263</v>
       </c>
     </row>
     <row r="31" spans="1:4" x14ac:dyDescent="0.25">
@@ -1615,7 +1608,7 @@
         <v>63</v>
       </c>
       <c r="D31" t="s">
-        <v>232</v>
+        <v>264</v>
       </c>
     </row>
     <row r="32" spans="1:4" x14ac:dyDescent="0.25">
@@ -1626,7 +1619,7 @@
         <v>14</v>
       </c>
       <c r="C32" t="s">
-        <v>233</v>
+        <v>232</v>
       </c>
       <c r="D32" t="s">
         <v>230</v>
@@ -1643,7 +1636,7 @@
         <v>181</v>
       </c>
       <c r="D33" t="s">
-        <v>232</v>
+        <v>264</v>
       </c>
     </row>
     <row r="34" spans="1:4" x14ac:dyDescent="0.25">
@@ -1654,7 +1647,7 @@
         <v>13</v>
       </c>
       <c r="C34" t="s">
-        <v>233</v>
+        <v>232</v>
       </c>
       <c r="D34" t="s">
         <v>230</v>
@@ -1696,7 +1689,7 @@
         <v>12</v>
       </c>
       <c r="C37" t="s">
-        <v>247</v>
+        <v>246</v>
       </c>
       <c r="D37" t="s">
         <v>230</v>
@@ -1713,7 +1706,7 @@
         <v>33</v>
       </c>
       <c r="D38" t="s">
-        <v>260</v>
+        <v>263</v>
       </c>
     </row>
     <row r="39" spans="1:4" x14ac:dyDescent="0.25">
@@ -1741,7 +1734,7 @@
         <v>55</v>
       </c>
       <c r="D40" t="s">
-        <v>235</v>
+        <v>234</v>
       </c>
     </row>
     <row r="41" spans="1:4" x14ac:dyDescent="0.25">
@@ -1766,10 +1759,10 @@
         <v>10</v>
       </c>
       <c r="C42" t="s">
-        <v>248</v>
+        <v>247</v>
       </c>
       <c r="D42" t="s">
-        <v>255</v>
+        <v>262</v>
       </c>
     </row>
     <row r="43" spans="1:4" x14ac:dyDescent="0.25">
@@ -1797,7 +1790,7 @@
         <v>74</v>
       </c>
       <c r="D44" t="s">
-        <v>260</v>
+        <v>263</v>
       </c>
     </row>
     <row r="45" spans="1:4" x14ac:dyDescent="0.25">
@@ -1811,7 +1804,7 @@
         <v>100</v>
       </c>
       <c r="D45" t="s">
-        <v>238</v>
+        <v>237</v>
       </c>
     </row>
     <row r="46" spans="1:4" x14ac:dyDescent="0.25">
@@ -1825,7 +1818,7 @@
         <v>173</v>
       </c>
       <c r="D46" t="s">
-        <v>255</v>
+        <v>262</v>
       </c>
     </row>
     <row r="47" spans="1:4" x14ac:dyDescent="0.25">
@@ -1839,7 +1832,7 @@
         <v>226</v>
       </c>
       <c r="D47" t="s">
-        <v>232</v>
+        <v>264</v>
       </c>
     </row>
     <row r="48" spans="1:4" x14ac:dyDescent="0.25">
@@ -1878,7 +1871,7 @@
         <v>7</v>
       </c>
       <c r="C50" t="s">
-        <v>233</v>
+        <v>232</v>
       </c>
       <c r="D50" t="s">
         <v>230</v>
@@ -1909,7 +1902,7 @@
         <v>35</v>
       </c>
       <c r="D52" t="s">
-        <v>235</v>
+        <v>234</v>
       </c>
     </row>
     <row r="53" spans="1:4" x14ac:dyDescent="0.25">
@@ -1923,7 +1916,7 @@
         <v>71</v>
       </c>
       <c r="D53" t="s">
-        <v>260</v>
+        <v>263</v>
       </c>
     </row>
     <row r="54" spans="1:4" x14ac:dyDescent="0.25">
@@ -1976,7 +1969,7 @@
         <v>6</v>
       </c>
       <c r="C57" t="s">
-        <v>233</v>
+        <v>232</v>
       </c>
       <c r="D57" t="s">
         <v>230</v>
@@ -1993,7 +1986,7 @@
         <v>158</v>
       </c>
       <c r="D58" t="s">
-        <v>260</v>
+        <v>263</v>
       </c>
     </row>
     <row r="59" spans="1:4" x14ac:dyDescent="0.25">
@@ -2035,7 +2028,7 @@
         <v>181</v>
       </c>
       <c r="D61" t="s">
-        <v>232</v>
+        <v>264</v>
       </c>
     </row>
     <row r="62" spans="1:4" x14ac:dyDescent="0.25">
@@ -2049,7 +2042,7 @@
         <v>31</v>
       </c>
       <c r="D62" t="s">
-        <v>260</v>
+        <v>263</v>
       </c>
     </row>
     <row r="63" spans="1:4" x14ac:dyDescent="0.25">
@@ -2063,7 +2056,7 @@
         <v>41</v>
       </c>
       <c r="D63" t="s">
-        <v>255</v>
+        <v>262</v>
       </c>
     </row>
     <row r="64" spans="1:4" x14ac:dyDescent="0.25">
@@ -2105,7 +2098,7 @@
         <v>91</v>
       </c>
       <c r="D66" t="s">
-        <v>235</v>
+        <v>234</v>
       </c>
     </row>
     <row r="67" spans="1:4" x14ac:dyDescent="0.25">
@@ -2175,7 +2168,7 @@
         <v>8</v>
       </c>
       <c r="D71" t="s">
-        <v>260</v>
+        <v>263</v>
       </c>
     </row>
     <row r="72" spans="1:4" x14ac:dyDescent="0.25">
@@ -2189,7 +2182,7 @@
         <v>34</v>
       </c>
       <c r="D72" t="s">
-        <v>235</v>
+        <v>234</v>
       </c>
     </row>
     <row r="73" spans="1:4" x14ac:dyDescent="0.25">
@@ -2203,7 +2196,7 @@
         <v>181</v>
       </c>
       <c r="D73" t="s">
-        <v>232</v>
+        <v>264</v>
       </c>
     </row>
     <row r="74" spans="1:4" x14ac:dyDescent="0.25">
@@ -2231,7 +2224,7 @@
         <v>80</v>
       </c>
       <c r="D75" t="s">
-        <v>235</v>
+        <v>234</v>
       </c>
     </row>
     <row r="76" spans="1:4" x14ac:dyDescent="0.25">
@@ -2245,7 +2238,7 @@
         <v>98</v>
       </c>
       <c r="D76" t="s">
-        <v>238</v>
+        <v>237</v>
       </c>
     </row>
     <row r="77" spans="1:4" x14ac:dyDescent="0.25">
@@ -2259,7 +2252,7 @@
         <v>107</v>
       </c>
       <c r="D77" t="s">
-        <v>235</v>
+        <v>234</v>
       </c>
     </row>
     <row r="78" spans="1:4" x14ac:dyDescent="0.25">
@@ -2326,7 +2319,7 @@
         <v>4</v>
       </c>
       <c r="C82" t="s">
-        <v>250</v>
+        <v>249</v>
       </c>
       <c r="D82" t="s">
         <v>230</v>
@@ -2343,7 +2336,7 @@
         <v>146</v>
       </c>
       <c r="D83" t="s">
-        <v>235</v>
+        <v>234</v>
       </c>
     </row>
     <row r="84" spans="1:4" x14ac:dyDescent="0.25">
@@ -2354,10 +2347,10 @@
         <v>4</v>
       </c>
       <c r="C84" t="s">
-        <v>253</v>
+        <v>252</v>
       </c>
       <c r="D84" t="s">
-        <v>260</v>
+        <v>263</v>
       </c>
     </row>
     <row r="85" spans="1:4" x14ac:dyDescent="0.25">
@@ -2371,7 +2364,7 @@
         <v>181</v>
       </c>
       <c r="D85" t="s">
-        <v>232</v>
+        <v>264</v>
       </c>
     </row>
     <row r="86" spans="1:4" x14ac:dyDescent="0.25">
@@ -2396,10 +2389,10 @@
         <v>4</v>
       </c>
       <c r="C87" t="s">
-        <v>254</v>
+        <v>253</v>
       </c>
       <c r="D87" t="s">
-        <v>255</v>
+        <v>262</v>
       </c>
     </row>
     <row r="88" spans="1:4" x14ac:dyDescent="0.25">
@@ -2410,10 +2403,10 @@
         <v>4</v>
       </c>
       <c r="C88" t="s">
-        <v>249</v>
+        <v>248</v>
       </c>
       <c r="D88" t="s">
-        <v>255</v>
+        <v>262</v>
       </c>
     </row>
     <row r="89" spans="1:4" x14ac:dyDescent="0.25">
@@ -2424,7 +2417,7 @@
         <v>3</v>
       </c>
       <c r="C89" t="s">
-        <v>246</v>
+        <v>245</v>
       </c>
       <c r="D89" t="s">
         <v>221</v>
@@ -2455,7 +2448,7 @@
         <v>26</v>
       </c>
       <c r="D91" t="s">
-        <v>260</v>
+        <v>263</v>
       </c>
     </row>
     <row r="92" spans="1:4" x14ac:dyDescent="0.25">
@@ -2469,7 +2462,7 @@
         <v>36</v>
       </c>
       <c r="D92" t="s">
-        <v>232</v>
+        <v>264</v>
       </c>
     </row>
     <row r="93" spans="1:4" x14ac:dyDescent="0.25">
@@ -2483,7 +2476,7 @@
         <v>38</v>
       </c>
       <c r="D93" t="s">
-        <v>235</v>
+        <v>234</v>
       </c>
     </row>
     <row r="94" spans="1:4" x14ac:dyDescent="0.25">
@@ -2511,7 +2504,7 @@
         <v>72</v>
       </c>
       <c r="D95" t="s">
-        <v>235</v>
+        <v>234</v>
       </c>
     </row>
     <row r="96" spans="1:4" x14ac:dyDescent="0.25">
@@ -2606,7 +2599,7 @@
         <v>3</v>
       </c>
       <c r="C102" t="s">
-        <v>263</v>
+        <v>259</v>
       </c>
       <c r="D102" t="s">
         <v>230</v>
@@ -2620,10 +2613,10 @@
         <v>3</v>
       </c>
       <c r="C103" t="s">
-        <v>258</v>
+        <v>256</v>
       </c>
       <c r="D103" t="s">
-        <v>255</v>
+        <v>262</v>
       </c>
     </row>
     <row r="104" spans="1:4" x14ac:dyDescent="0.25">
@@ -2648,10 +2641,10 @@
         <v>3</v>
       </c>
       <c r="C105" t="s">
-        <v>257</v>
+        <v>255</v>
       </c>
       <c r="D105" t="s">
-        <v>232</v>
+        <v>264</v>
       </c>
     </row>
     <row r="106" spans="1:4" x14ac:dyDescent="0.25">
@@ -2665,7 +2658,7 @@
         <v>181</v>
       </c>
       <c r="D106" t="s">
-        <v>232</v>
+        <v>264</v>
       </c>
     </row>
     <row r="107" spans="1:4" x14ac:dyDescent="0.25">
@@ -2676,7 +2669,7 @@
         <v>3</v>
       </c>
       <c r="C107" t="s">
-        <v>246</v>
+        <v>245</v>
       </c>
       <c r="D107" t="s">
         <v>221</v>
@@ -2690,10 +2683,10 @@
         <v>3</v>
       </c>
       <c r="C108" t="s">
-        <v>248</v>
+        <v>247</v>
       </c>
       <c r="D108" t="s">
-        <v>255</v>
+        <v>262</v>
       </c>
     </row>
     <row r="109" spans="1:4" x14ac:dyDescent="0.25">
@@ -2704,10 +2697,10 @@
         <v>3</v>
       </c>
       <c r="C109" t="s">
-        <v>256</v>
+        <v>254</v>
       </c>
       <c r="D109" t="s">
-        <v>255</v>
+        <v>262</v>
       </c>
     </row>
     <row r="110" spans="1:4" x14ac:dyDescent="0.25">
@@ -2718,10 +2711,10 @@
         <v>3</v>
       </c>
       <c r="C110" t="s">
-        <v>249</v>
+        <v>248</v>
       </c>
       <c r="D110" t="s">
-        <v>255</v>
+        <v>262</v>
       </c>
     </row>
     <row r="111" spans="1:4" x14ac:dyDescent="0.25">
@@ -2760,7 +2753,7 @@
         <v>2</v>
       </c>
       <c r="C113" t="s">
-        <v>234</v>
+        <v>233</v>
       </c>
       <c r="D113" t="s">
         <v>230</v>
@@ -2774,10 +2767,10 @@
         <v>2</v>
       </c>
       <c r="C114" t="s">
-        <v>253</v>
+        <v>252</v>
       </c>
       <c r="D114" t="s">
-        <v>260</v>
+        <v>263</v>
       </c>
     </row>
     <row r="115" spans="1:4" x14ac:dyDescent="0.25">
@@ -2816,10 +2809,10 @@
         <v>2</v>
       </c>
       <c r="C117" t="s">
-        <v>236</v>
+        <v>235</v>
       </c>
       <c r="D117" t="s">
-        <v>235</v>
+        <v>234</v>
       </c>
     </row>
     <row r="118" spans="1:4" x14ac:dyDescent="0.25">
@@ -2830,10 +2823,10 @@
         <v>2</v>
       </c>
       <c r="C118" t="s">
-        <v>237</v>
+        <v>236</v>
       </c>
       <c r="D118" t="s">
-        <v>235</v>
+        <v>234</v>
       </c>
     </row>
     <row r="119" spans="1:4" x14ac:dyDescent="0.25">
@@ -2847,7 +2840,7 @@
         <v>26</v>
       </c>
       <c r="D119" t="s">
-        <v>260</v>
+        <v>263</v>
       </c>
     </row>
     <row r="120" spans="1:4" x14ac:dyDescent="0.25">
@@ -2861,7 +2854,7 @@
         <v>87</v>
       </c>
       <c r="D120" t="s">
-        <v>260</v>
+        <v>263</v>
       </c>
     </row>
     <row r="121" spans="1:4" x14ac:dyDescent="0.25">
@@ -2875,7 +2868,7 @@
         <v>76</v>
       </c>
       <c r="D121" t="s">
-        <v>235</v>
+        <v>234</v>
       </c>
     </row>
     <row r="122" spans="1:4" x14ac:dyDescent="0.25">
@@ -2889,7 +2882,7 @@
         <v>77</v>
       </c>
       <c r="D122" t="s">
-        <v>235</v>
+        <v>234</v>
       </c>
     </row>
     <row r="123" spans="1:4" x14ac:dyDescent="0.25">
@@ -2900,7 +2893,7 @@
         <v>2</v>
       </c>
       <c r="C123" t="s">
-        <v>233</v>
+        <v>232</v>
       </c>
       <c r="D123" t="s">
         <v>230</v>
@@ -2928,7 +2921,7 @@
         <v>2</v>
       </c>
       <c r="C125" t="s">
-        <v>259</v>
+        <v>257</v>
       </c>
       <c r="D125" t="s">
         <v>229</v>
@@ -2945,7 +2938,7 @@
         <v>86</v>
       </c>
       <c r="D126" t="s">
-        <v>255</v>
+        <v>262</v>
       </c>
     </row>
     <row r="127" spans="1:4" x14ac:dyDescent="0.25">
@@ -2959,7 +2952,7 @@
         <v>87</v>
       </c>
       <c r="D127" t="s">
-        <v>260</v>
+        <v>263</v>
       </c>
     </row>
     <row r="128" spans="1:4" x14ac:dyDescent="0.25">
@@ -2987,7 +2980,7 @@
         <v>93</v>
       </c>
       <c r="D129" t="s">
-        <v>260</v>
+        <v>263</v>
       </c>
     </row>
     <row r="130" spans="1:4" x14ac:dyDescent="0.25">
@@ -3001,7 +2994,7 @@
         <v>96</v>
       </c>
       <c r="D130" t="s">
-        <v>255</v>
+        <v>262</v>
       </c>
     </row>
     <row r="131" spans="1:4" x14ac:dyDescent="0.25">
@@ -3127,7 +3120,7 @@
         <v>148</v>
       </c>
       <c r="D139" t="s">
-        <v>260</v>
+        <v>263</v>
       </c>
     </row>
     <row r="140" spans="1:4" x14ac:dyDescent="0.25">
@@ -3141,7 +3134,7 @@
         <v>155</v>
       </c>
       <c r="D140" t="s">
-        <v>232</v>
+        <v>264</v>
       </c>
     </row>
     <row r="141" spans="1:4" x14ac:dyDescent="0.25">
@@ -3152,10 +3145,10 @@
         <v>2</v>
       </c>
       <c r="C141" t="s">
-        <v>257</v>
+        <v>255</v>
       </c>
       <c r="D141" t="s">
-        <v>232</v>
+        <v>264</v>
       </c>
     </row>
     <row r="142" spans="1:4" x14ac:dyDescent="0.25">
@@ -3169,7 +3162,7 @@
         <v>171</v>
       </c>
       <c r="D142" t="s">
-        <v>255</v>
+        <v>262</v>
       </c>
     </row>
     <row r="143" spans="1:4" x14ac:dyDescent="0.25">
@@ -3194,10 +3187,10 @@
         <v>2</v>
       </c>
       <c r="C144" t="s">
-        <v>243</v>
+        <v>242</v>
       </c>
       <c r="D144" t="s">
-        <v>255</v>
+        <v>262</v>
       </c>
     </row>
     <row r="145" spans="1:4" x14ac:dyDescent="0.25">
@@ -3222,7 +3215,7 @@
         <v>2</v>
       </c>
       <c r="C146" t="s">
-        <v>246</v>
+        <v>245</v>
       </c>
       <c r="D146" t="s">
         <v>221</v>
@@ -3250,10 +3243,10 @@
         <v>2</v>
       </c>
       <c r="C148" t="s">
-        <v>261</v>
+        <v>258</v>
       </c>
       <c r="D148" t="s">
-        <v>232</v>
+        <v>264</v>
       </c>
     </row>
     <row r="149" spans="1:4" x14ac:dyDescent="0.25">
@@ -3264,7 +3257,7 @@
         <v>1</v>
       </c>
       <c r="C149" t="s">
-        <v>233</v>
+        <v>232</v>
       </c>
       <c r="D149" t="s">
         <v>230</v>
@@ -3278,7 +3271,7 @@
         <v>1</v>
       </c>
       <c r="C150" t="s">
-        <v>233</v>
+        <v>232</v>
       </c>
       <c r="D150" t="s">
         <v>230</v>
@@ -3292,7 +3285,7 @@
         <v>1</v>
       </c>
       <c r="C151" t="s">
-        <v>233</v>
+        <v>232</v>
       </c>
       <c r="D151" t="s">
         <v>230</v>
@@ -3334,7 +3327,7 @@
         <v>1</v>
       </c>
       <c r="C154" t="s">
-        <v>233</v>
+        <v>232</v>
       </c>
       <c r="D154" t="s">
         <v>230</v>
@@ -3376,7 +3369,7 @@
         <v>1</v>
       </c>
       <c r="C157" t="s">
-        <v>240</v>
+        <v>239</v>
       </c>
       <c r="D157" t="s">
         <v>230</v>
@@ -3393,7 +3386,7 @@
         <v>19</v>
       </c>
       <c r="D158" t="s">
-        <v>255</v>
+        <v>262</v>
       </c>
     </row>
     <row r="159" spans="1:4" x14ac:dyDescent="0.25">
@@ -3404,10 +3397,10 @@
         <v>1</v>
       </c>
       <c r="C159" t="s">
-        <v>239</v>
+        <v>238</v>
       </c>
       <c r="D159" t="s">
-        <v>238</v>
+        <v>237</v>
       </c>
     </row>
     <row r="160" spans="1:4" x14ac:dyDescent="0.25">
@@ -3418,10 +3411,10 @@
         <v>1</v>
       </c>
       <c r="C160" t="s">
-        <v>239</v>
+        <v>238</v>
       </c>
       <c r="D160" t="s">
-        <v>238</v>
+        <v>237</v>
       </c>
     </row>
     <row r="161" spans="1:4" x14ac:dyDescent="0.25">
@@ -3435,7 +3428,7 @@
         <v>226</v>
       </c>
       <c r="D161" t="s">
-        <v>232</v>
+        <v>264</v>
       </c>
     </row>
     <row r="162" spans="1:4" x14ac:dyDescent="0.25">
@@ -3449,7 +3442,7 @@
         <v>181</v>
       </c>
       <c r="D162" t="s">
-        <v>232</v>
+        <v>264</v>
       </c>
     </row>
     <row r="163" spans="1:4" x14ac:dyDescent="0.25">
@@ -3505,7 +3498,7 @@
         <v>226</v>
       </c>
       <c r="D166" t="s">
-        <v>232</v>
+        <v>264</v>
       </c>
     </row>
     <row r="167" spans="1:4" x14ac:dyDescent="0.25">
@@ -3544,7 +3537,7 @@
         <v>1</v>
       </c>
       <c r="C169" t="s">
-        <v>234</v>
+        <v>233</v>
       </c>
       <c r="D169" t="s">
         <v>230</v>
@@ -3561,7 +3554,7 @@
         <v>55</v>
       </c>
       <c r="D170" t="s">
-        <v>235</v>
+        <v>234</v>
       </c>
     </row>
     <row r="171" spans="1:4" x14ac:dyDescent="0.25">
@@ -3586,10 +3579,10 @@
         <v>1</v>
       </c>
       <c r="C172" t="s">
-        <v>261</v>
+        <v>258</v>
       </c>
       <c r="D172" t="s">
-        <v>232</v>
+        <v>264</v>
       </c>
     </row>
     <row r="173" spans="1:4" x14ac:dyDescent="0.25">
@@ -3600,7 +3593,7 @@
         <v>1</v>
       </c>
       <c r="C173" t="s">
-        <v>262</v>
+        <v>240</v>
       </c>
       <c r="D173" t="s">
         <v>228</v>
@@ -3614,10 +3607,10 @@
         <v>1</v>
       </c>
       <c r="C174" t="s">
-        <v>253</v>
+        <v>252</v>
       </c>
       <c r="D174" t="s">
-        <v>260</v>
+        <v>263</v>
       </c>
     </row>
     <row r="175" spans="1:4" x14ac:dyDescent="0.25">
@@ -3642,10 +3635,10 @@
         <v>1</v>
       </c>
       <c r="C176" t="s">
-        <v>264</v>
+        <v>260</v>
       </c>
       <c r="D176" t="s">
-        <v>260</v>
+        <v>263</v>
       </c>
     </row>
     <row r="177" spans="1:4" x14ac:dyDescent="0.25">
@@ -3656,10 +3649,10 @@
         <v>1</v>
       </c>
       <c r="C177" t="s">
-        <v>264</v>
+        <v>260</v>
       </c>
       <c r="D177" t="s">
-        <v>260</v>
+        <v>263</v>
       </c>
     </row>
     <row r="178" spans="1:4" x14ac:dyDescent="0.25">
@@ -3670,10 +3663,10 @@
         <v>1</v>
       </c>
       <c r="C178" t="s">
-        <v>261</v>
+        <v>258</v>
       </c>
       <c r="D178" t="s">
-        <v>232</v>
+        <v>264</v>
       </c>
     </row>
     <row r="179" spans="1:4" x14ac:dyDescent="0.25">
@@ -3687,7 +3680,7 @@
         <v>181</v>
       </c>
       <c r="D179" t="s">
-        <v>232</v>
+        <v>264</v>
       </c>
     </row>
     <row r="180" spans="1:4" x14ac:dyDescent="0.25">
@@ -3701,7 +3694,7 @@
         <v>155</v>
       </c>
       <c r="D180" t="s">
-        <v>232</v>
+        <v>264</v>
       </c>
     </row>
     <row r="181" spans="1:4" x14ac:dyDescent="0.25">
@@ -3712,10 +3705,10 @@
         <v>1</v>
       </c>
       <c r="C181" t="s">
-        <v>257</v>
+        <v>255</v>
       </c>
       <c r="D181" t="s">
-        <v>232</v>
+        <v>264</v>
       </c>
     </row>
     <row r="182" spans="1:4" x14ac:dyDescent="0.25">
@@ -3754,10 +3747,10 @@
         <v>1</v>
       </c>
       <c r="C184" t="s">
-        <v>264</v>
+        <v>260</v>
       </c>
       <c r="D184" t="s">
-        <v>260</v>
+        <v>263</v>
       </c>
     </row>
     <row r="185" spans="1:4" x14ac:dyDescent="0.25">
@@ -3768,10 +3761,10 @@
         <v>1</v>
       </c>
       <c r="C185" t="s">
-        <v>251</v>
+        <v>250</v>
       </c>
       <c r="D185" t="s">
-        <v>255</v>
+        <v>262</v>
       </c>
     </row>
     <row r="186" spans="1:4" x14ac:dyDescent="0.25">
@@ -3785,7 +3778,7 @@
         <v>36</v>
       </c>
       <c r="D186" t="s">
-        <v>232</v>
+        <v>264</v>
       </c>
     </row>
     <row r="187" spans="1:4" x14ac:dyDescent="0.25">
@@ -3796,10 +3789,10 @@
         <v>1</v>
       </c>
       <c r="C187" t="s">
-        <v>239</v>
+        <v>238</v>
       </c>
       <c r="D187" t="s">
-        <v>238</v>
+        <v>237</v>
       </c>
     </row>
     <row r="188" spans="1:4" x14ac:dyDescent="0.25">
@@ -3810,7 +3803,7 @@
         <v>1</v>
       </c>
       <c r="C188" t="s">
-        <v>233</v>
+        <v>232</v>
       </c>
       <c r="D188" t="s">
         <v>230</v>
@@ -3869,7 +3862,7 @@
         <v>173</v>
       </c>
       <c r="D192" t="s">
-        <v>255</v>
+        <v>262</v>
       </c>
     </row>
     <row r="193" spans="1:4" x14ac:dyDescent="0.25">
@@ -3880,7 +3873,7 @@
         <v>1</v>
       </c>
       <c r="C193" t="s">
-        <v>263</v>
+        <v>259</v>
       </c>
       <c r="D193" t="s">
         <v>230</v>
@@ -3894,7 +3887,7 @@
         <v>1</v>
       </c>
       <c r="C194" t="s">
-        <v>250</v>
+        <v>249</v>
       </c>
       <c r="D194" t="s">
         <v>230</v>
@@ -3908,7 +3901,7 @@
         <v>1</v>
       </c>
       <c r="C195" t="s">
-        <v>250</v>
+        <v>249</v>
       </c>
       <c r="D195" t="s">
         <v>230</v>
@@ -3922,7 +3915,7 @@
         <v>1</v>
       </c>
       <c r="C196" t="s">
-        <v>250</v>
+        <v>249</v>
       </c>
       <c r="D196" t="s">
         <v>230</v>
@@ -3950,7 +3943,7 @@
         <v>1</v>
       </c>
       <c r="C198" t="s">
-        <v>263</v>
+        <v>259</v>
       </c>
       <c r="D198" t="s">
         <v>230</v>
@@ -3964,7 +3957,7 @@
         <v>1</v>
       </c>
       <c r="C199" t="s">
-        <v>263</v>
+        <v>259</v>
       </c>
       <c r="D199" t="s">
         <v>230</v>
@@ -3978,7 +3971,7 @@
         <v>1</v>
       </c>
       <c r="C200" t="s">
-        <v>250</v>
+        <v>249</v>
       </c>
       <c r="D200" t="s">
         <v>230</v>
@@ -3992,7 +3985,7 @@
         <v>1</v>
       </c>
       <c r="C201" t="s">
-        <v>250</v>
+        <v>249</v>
       </c>
       <c r="D201" t="s">
         <v>230</v>
@@ -4009,7 +4002,7 @@
         <v>155</v>
       </c>
       <c r="D202" t="s">
-        <v>232</v>
+        <v>264</v>
       </c>
     </row>
     <row r="203" spans="1:4" x14ac:dyDescent="0.25">
@@ -4020,7 +4013,7 @@
         <v>1</v>
       </c>
       <c r="C203" t="s">
-        <v>233</v>
+        <v>232</v>
       </c>
       <c r="D203" t="s">
         <v>230</v>
@@ -4034,10 +4027,10 @@
         <v>1</v>
       </c>
       <c r="C204" t="s">
-        <v>264</v>
+        <v>260</v>
       </c>
       <c r="D204" t="s">
-        <v>260</v>
+        <v>263</v>
       </c>
     </row>
     <row r="205" spans="1:4" x14ac:dyDescent="0.25">
@@ -4048,10 +4041,10 @@
         <v>1</v>
       </c>
       <c r="C205" t="s">
-        <v>264</v>
+        <v>260</v>
       </c>
       <c r="D205" t="s">
-        <v>260</v>
+        <v>263</v>
       </c>
     </row>
     <row r="206" spans="1:4" x14ac:dyDescent="0.25">
@@ -4065,7 +4058,7 @@
         <v>164</v>
       </c>
       <c r="D206" t="s">
-        <v>255</v>
+        <v>262</v>
       </c>
     </row>
     <row r="207" spans="1:4" x14ac:dyDescent="0.25">
@@ -4093,7 +4086,7 @@
         <v>155</v>
       </c>
       <c r="D208" t="s">
-        <v>232</v>
+        <v>264</v>
       </c>
     </row>
     <row r="209" spans="1:4" x14ac:dyDescent="0.25">
@@ -4107,7 +4100,7 @@
         <v>155</v>
       </c>
       <c r="D209" t="s">
-        <v>232</v>
+        <v>264</v>
       </c>
     </row>
     <row r="210" spans="1:4" x14ac:dyDescent="0.25">
@@ -4121,7 +4114,7 @@
         <v>155</v>
       </c>
       <c r="D210" t="s">
-        <v>232</v>
+        <v>264</v>
       </c>
     </row>
     <row r="211" spans="1:4" x14ac:dyDescent="0.25">
@@ -4135,7 +4128,7 @@
         <v>155</v>
       </c>
       <c r="D211" t="s">
-        <v>232</v>
+        <v>264</v>
       </c>
     </row>
     <row r="212" spans="1:4" x14ac:dyDescent="0.25">
@@ -4149,7 +4142,7 @@
         <v>155</v>
       </c>
       <c r="D212" t="s">
-        <v>232</v>
+        <v>264</v>
       </c>
     </row>
     <row r="213" spans="1:4" x14ac:dyDescent="0.25">
@@ -4163,7 +4156,7 @@
         <v>181</v>
       </c>
       <c r="D213" t="s">
-        <v>232</v>
+        <v>264</v>
       </c>
     </row>
     <row r="214" spans="1:4" x14ac:dyDescent="0.25">
@@ -4174,10 +4167,10 @@
         <v>1</v>
       </c>
       <c r="C214" t="s">
-        <v>257</v>
+        <v>255</v>
       </c>
       <c r="D214" t="s">
-        <v>232</v>
+        <v>264</v>
       </c>
     </row>
     <row r="215" spans="1:4" x14ac:dyDescent="0.25">
@@ -4188,10 +4181,10 @@
         <v>1</v>
       </c>
       <c r="C215" t="s">
-        <v>261</v>
+        <v>258</v>
       </c>
       <c r="D215" t="s">
-        <v>232</v>
+        <v>264</v>
       </c>
     </row>
     <row r="216" spans="1:4" x14ac:dyDescent="0.25">
@@ -4219,7 +4212,7 @@
         <v>173</v>
       </c>
       <c r="D217" t="s">
-        <v>255</v>
+        <v>262</v>
       </c>
     </row>
     <row r="218" spans="1:4" x14ac:dyDescent="0.25">
@@ -4230,10 +4223,10 @@
         <v>1</v>
       </c>
       <c r="C218" t="s">
-        <v>251</v>
+        <v>250</v>
       </c>
       <c r="D218" t="s">
-        <v>255</v>
+        <v>262</v>
       </c>
     </row>
     <row r="219" spans="1:4" x14ac:dyDescent="0.25">
@@ -4258,10 +4251,10 @@
         <v>1</v>
       </c>
       <c r="C220" t="s">
-        <v>251</v>
+        <v>250</v>
       </c>
       <c r="D220" t="s">
-        <v>255</v>
+        <v>262</v>
       </c>
     </row>
     <row r="221" spans="1:4" x14ac:dyDescent="0.25">
@@ -4275,18 +4268,18 @@
         <v>173</v>
       </c>
       <c r="D221" t="s">
-        <v>255</v>
+        <v>262</v>
       </c>
     </row>
     <row r="222" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A222" t="s">
-        <v>265</v>
+        <v>261</v>
       </c>
       <c r="B222">
         <v>1</v>
       </c>
       <c r="C222" t="s">
-        <v>233</v>
+        <v>232</v>
       </c>
       <c r="D222" t="s">
         <v>230</v>

</xml_diff>

<commit_message>
app interactive ego reseau
</commit_message>
<xml_diff>
--- a/data/intermediate/reseau/recategorize_designation.xlsx
+++ b/data/intermediate/reseau/recategorize_designation.xlsx
@@ -8,19 +8,32 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://genes-my.sharepoint.com/personal/lmaurice_ensae_fr/Documents/CCNE/Analyse/CCNE/data/intermediate/reseau/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="610" documentId="11_B89231273C696DEBE4B4ADE2E75D06D0725D8531" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{5D20DBC1-B9B3-473A-834A-FC92FFA503E9}"/>
+  <xr:revisionPtr revIDLastSave="688" documentId="11_B89231273C696DEBE4B4ADE2E75D06D0725D8531" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{FDD1E397-9E8B-403B-AC40-147ACA0DBE64}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15720" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="19090" yWindow="-940" windowWidth="22620" windowHeight="13500" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet 1" sheetId="1" r:id="rId1"/>
   </sheets>
-  <calcPr calcId="0"/>
+  <calcPr calcId="191029"/>
+  <extLst>
+    <ext xmlns:xcalcf="http://schemas.microsoft.com/office/spreadsheetml/2018/calcfeatures" uri="{B58B0392-4F1F-4190-BB64-5DF3571DCE5F}">
+      <xcalcf:calcFeatures>
+        <xcalcf:feature name="microsoft.com:RD"/>
+        <xcalcf:feature name="microsoft.com:Single"/>
+        <xcalcf:feature name="microsoft.com:FV"/>
+        <xcalcf:feature name="microsoft.com:CNMTM"/>
+        <xcalcf:feature name="microsoft.com:LET_WF"/>
+        <xcalcf:feature name="microsoft.com:LAMBDA_WF"/>
+        <xcalcf:feature name="microsoft.com:ARRAYTEXT_WF"/>
+      </xcalcf:calcFeatures>
+    </ext>
+  </extLst>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="667" uniqueCount="265">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="727" uniqueCount="287">
   <si>
     <t>Désignation</t>
   </si>
@@ -815,6 +828,72 @@
   </si>
   <si>
     <t>Org Internationales</t>
+  </si>
+  <si>
+    <t>Conseil des organisations internationales des sciences médicales</t>
+  </si>
+  <si>
+    <t>Déclaration d'Helsinki</t>
+  </si>
+  <si>
+    <t>Centre national de transfusion sanguine</t>
+  </si>
+  <si>
+    <t>Espagne</t>
+  </si>
+  <si>
+    <t>Italie</t>
+  </si>
+  <si>
+    <t>COPE</t>
+  </si>
+  <si>
+    <t>Brazilian Institutions</t>
+  </si>
+  <si>
+    <t>Code procédure pénale</t>
+  </si>
+  <si>
+    <t>Loi du 17 janvier 1975 (Veil)</t>
+  </si>
+  <si>
+    <t>Loi du 17 janvier 1975 (Veil)</t>
+  </si>
+  <si>
+    <t>Loi du 22 décembre 1976 (Caillavet)</t>
+  </si>
+  <si>
+    <t>Cour de cassation</t>
+  </si>
+  <si>
+    <t>Mtravail</t>
+  </si>
+  <si>
+    <t>Loi du 31 décembre 1970</t>
+  </si>
+  <si>
+    <t>Ministères Sociaux</t>
+  </si>
+  <si>
+    <t>INSERM/CNRS</t>
+  </si>
+  <si>
+    <t>CNRS</t>
+  </si>
+  <si>
+    <t>CIO</t>
+  </si>
+  <si>
+    <t>Org Inter divers</t>
+  </si>
+  <si>
+    <t>Déclaration d'Helsinki et de Manille</t>
+  </si>
+  <si>
+    <t>Bourdieu</t>
+  </si>
+  <si>
+    <t>Code de procédure pénale</t>
   </si>
 </sst>
 </file>
@@ -869,11 +948,15 @@
 </styleSheet>
 </file>
 
+<file path=xl/persons/person.xml><?xml version="1.0" encoding="utf-8"?>
+<personList xmlns="http://schemas.microsoft.com/office/spreadsheetml/2018/threadedcomments" xmlns:x="http://schemas.openxmlformats.org/spreadsheetml/2006/main"/>
+</file>
+
 <file path=xl/tables/table1.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="1" xr:uid="{74E48EA6-D00C-44C7-827C-672438CB5CD0}" name="Tableau1" displayName="Tableau1" ref="A1:D1048574" totalsRowShown="0">
-  <autoFilter ref="A1:D1048574" xr:uid="{74E48EA6-D00C-44C7-827C-672438CB5CD0}"/>
-  <sortState xmlns:xlrd2="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata2" ref="A2:D1048574">
-    <sortCondition descending="1" ref="B1:B1048574"/>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="1" xr:uid="{74E48EA6-D00C-44C7-827C-672438CB5CD0}" name="Tableau1" displayName="Tableau1" ref="A1:D1048575" totalsRowShown="0">
+  <autoFilter ref="A1:D1048575" xr:uid="{74E48EA6-D00C-44C7-827C-672438CB5CD0}"/>
+  <sortState xmlns:xlrd2="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata2" ref="A2:D1048575">
+    <sortCondition descending="1" ref="B1:B1048575"/>
   </sortState>
   <tableColumns count="4">
     <tableColumn id="1" xr3:uid="{2536FB48-B587-4C50-8117-0D0C34C6FE51}" name="Désignation"/>
@@ -1164,10 +1247,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:D222"/>
+  <dimension ref="A1:D242"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A35" workbookViewId="0">
-      <selection activeCell="I50" sqref="I50"/>
+    <sheetView tabSelected="1" topLeftCell="A233" workbookViewId="0">
+      <selection activeCell="A241" sqref="A241"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1801,7 +1884,7 @@
         <v>8</v>
       </c>
       <c r="C45" t="s">
-        <v>100</v>
+        <v>280</v>
       </c>
       <c r="D45" t="s">
         <v>237</v>
@@ -3573,13 +3656,13 @@
     </row>
     <row r="172" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A172" t="s">
-        <v>48</v>
+        <v>284</v>
       </c>
       <c r="B172">
-        <v>1</v>
+        <v>5</v>
       </c>
       <c r="C172" t="s">
-        <v>258</v>
+        <v>284</v>
       </c>
       <c r="D172" t="s">
         <v>264</v>
@@ -3587,63 +3670,63 @@
     </row>
     <row r="173" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A173" t="s">
-        <v>49</v>
+        <v>48</v>
       </c>
       <c r="B173">
-        <v>1</v>
+        <v>5</v>
       </c>
       <c r="C173" t="s">
-        <v>240</v>
+        <v>48</v>
       </c>
       <c r="D173" t="s">
-        <v>228</v>
+        <v>264</v>
       </c>
     </row>
     <row r="174" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A174" t="s">
-        <v>57</v>
+        <v>49</v>
       </c>
       <c r="B174">
         <v>1</v>
       </c>
       <c r="C174" t="s">
-        <v>252</v>
+        <v>240</v>
       </c>
       <c r="D174" t="s">
-        <v>263</v>
+        <v>228</v>
       </c>
     </row>
     <row r="175" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A175" t="s">
-        <v>60</v>
+        <v>57</v>
       </c>
       <c r="B175">
         <v>1</v>
       </c>
       <c r="C175" t="s">
-        <v>168</v>
+        <v>252</v>
       </c>
       <c r="D175" t="s">
-        <v>230</v>
+        <v>263</v>
       </c>
     </row>
     <row r="176" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A176" t="s">
-        <v>65</v>
+        <v>60</v>
       </c>
       <c r="B176">
         <v>1</v>
       </c>
       <c r="C176" t="s">
-        <v>260</v>
+        <v>168</v>
       </c>
       <c r="D176" t="s">
-        <v>263</v>
+        <v>230</v>
       </c>
     </row>
     <row r="177" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A177" t="s">
-        <v>66</v>
+        <v>65</v>
       </c>
       <c r="B177">
         <v>1</v>
@@ -3657,27 +3740,27 @@
     </row>
     <row r="178" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A178" t="s">
-        <v>69</v>
+        <v>66</v>
       </c>
       <c r="B178">
         <v>1</v>
       </c>
       <c r="C178" t="s">
-        <v>258</v>
+        <v>260</v>
       </c>
       <c r="D178" t="s">
-        <v>264</v>
+        <v>263</v>
       </c>
     </row>
     <row r="179" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A179" t="s">
-        <v>81</v>
+        <v>69</v>
       </c>
       <c r="B179">
         <v>1</v>
       </c>
       <c r="C179" t="s">
-        <v>181</v>
+        <v>258</v>
       </c>
       <c r="D179" t="s">
         <v>264</v>
@@ -3685,13 +3768,13 @@
     </row>
     <row r="180" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A180" t="s">
-        <v>82</v>
+        <v>81</v>
       </c>
       <c r="B180">
         <v>1</v>
       </c>
       <c r="C180" t="s">
-        <v>155</v>
+        <v>181</v>
       </c>
       <c r="D180" t="s">
         <v>264</v>
@@ -3699,13 +3782,13 @@
     </row>
     <row r="181" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A181" t="s">
-        <v>83</v>
+        <v>82</v>
       </c>
       <c r="B181">
         <v>1</v>
       </c>
       <c r="C181" t="s">
-        <v>255</v>
+        <v>155</v>
       </c>
       <c r="D181" t="s">
         <v>264</v>
@@ -3713,181 +3796,181 @@
     </row>
     <row r="182" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A182" t="s">
-        <v>89</v>
+        <v>83</v>
       </c>
       <c r="B182">
         <v>1</v>
       </c>
       <c r="C182" t="s">
-        <v>222</v>
+        <v>255</v>
       </c>
       <c r="D182" t="s">
-        <v>230</v>
+        <v>264</v>
       </c>
     </row>
     <row r="183" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A183" t="s">
-        <v>90</v>
+        <v>89</v>
       </c>
       <c r="B183">
         <v>1</v>
       </c>
       <c r="C183" t="s">
-        <v>225</v>
+        <v>222</v>
       </c>
       <c r="D183" t="s">
-        <v>227</v>
+        <v>230</v>
       </c>
     </row>
     <row r="184" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A184" t="s">
-        <v>94</v>
+        <v>90</v>
       </c>
       <c r="B184">
         <v>1</v>
       </c>
       <c r="C184" t="s">
-        <v>260</v>
+        <v>225</v>
       </c>
       <c r="D184" t="s">
-        <v>263</v>
+        <v>227</v>
       </c>
     </row>
     <row r="185" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A185" t="s">
-        <v>97</v>
+        <v>94</v>
       </c>
       <c r="B185">
         <v>1</v>
       </c>
       <c r="C185" t="s">
-        <v>250</v>
+        <v>260</v>
       </c>
       <c r="D185" t="s">
-        <v>262</v>
+        <v>263</v>
       </c>
     </row>
     <row r="186" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A186" t="s">
-        <v>101</v>
+        <v>97</v>
       </c>
       <c r="B186">
         <v>1</v>
       </c>
       <c r="C186" t="s">
-        <v>36</v>
+        <v>250</v>
       </c>
       <c r="D186" t="s">
-        <v>264</v>
+        <v>262</v>
       </c>
     </row>
     <row r="187" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A187" t="s">
-        <v>102</v>
+        <v>101</v>
       </c>
       <c r="B187">
         <v>1</v>
       </c>
       <c r="C187" t="s">
-        <v>238</v>
+        <v>36</v>
       </c>
       <c r="D187" t="s">
-        <v>237</v>
+        <v>264</v>
       </c>
     </row>
     <row r="188" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A188" t="s">
-        <v>104</v>
+        <v>102</v>
       </c>
       <c r="B188">
         <v>1</v>
       </c>
       <c r="C188" t="s">
-        <v>232</v>
+        <v>238</v>
       </c>
       <c r="D188" t="s">
-        <v>230</v>
+        <v>237</v>
       </c>
     </row>
     <row r="189" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A189" t="s">
-        <v>105</v>
+        <v>104</v>
       </c>
       <c r="B189">
         <v>1</v>
       </c>
       <c r="C189" t="s">
-        <v>225</v>
+        <v>232</v>
       </c>
       <c r="D189" t="s">
-        <v>227</v>
+        <v>230</v>
       </c>
     </row>
     <row r="190" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A190" t="s">
-        <v>109</v>
+        <v>105</v>
       </c>
       <c r="B190">
         <v>1</v>
       </c>
       <c r="C190" t="s">
-        <v>167</v>
+        <v>225</v>
       </c>
       <c r="D190" t="s">
-        <v>221</v>
+        <v>227</v>
       </c>
     </row>
     <row r="191" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A191" t="s">
-        <v>128</v>
+        <v>109</v>
       </c>
       <c r="B191">
         <v>1</v>
       </c>
       <c r="C191" t="s">
-        <v>137</v>
+        <v>167</v>
       </c>
       <c r="D191" t="s">
-        <v>230</v>
+        <v>221</v>
       </c>
     </row>
     <row r="192" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A192" t="s">
-        <v>130</v>
+        <v>128</v>
       </c>
       <c r="B192">
         <v>1</v>
       </c>
       <c r="C192" t="s">
-        <v>173</v>
+        <v>137</v>
       </c>
       <c r="D192" t="s">
-        <v>262</v>
+        <v>230</v>
       </c>
     </row>
     <row r="193" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A193" t="s">
-        <v>131</v>
+        <v>130</v>
       </c>
       <c r="B193">
         <v>1</v>
       </c>
       <c r="C193" t="s">
-        <v>259</v>
+        <v>173</v>
       </c>
       <c r="D193" t="s">
-        <v>230</v>
+        <v>262</v>
       </c>
     </row>
     <row r="194" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A194" t="s">
-        <v>132</v>
+        <v>131</v>
       </c>
       <c r="B194">
         <v>1</v>
       </c>
       <c r="C194" t="s">
-        <v>249</v>
+        <v>259</v>
       </c>
       <c r="D194" t="s">
         <v>230</v>
@@ -3895,7 +3978,7 @@
     </row>
     <row r="195" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A195" t="s">
-        <v>133</v>
+        <v>132</v>
       </c>
       <c r="B195">
         <v>1</v>
@@ -3909,7 +3992,7 @@
     </row>
     <row r="196" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A196" t="s">
-        <v>134</v>
+        <v>133</v>
       </c>
       <c r="B196">
         <v>1</v>
@@ -3923,13 +4006,13 @@
     </row>
     <row r="197" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A197" t="s">
-        <v>136</v>
+        <v>134</v>
       </c>
       <c r="B197">
         <v>1</v>
       </c>
       <c r="C197" t="s">
-        <v>137</v>
+        <v>249</v>
       </c>
       <c r="D197" t="s">
         <v>230</v>
@@ -3937,13 +4020,13 @@
     </row>
     <row r="198" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A198" t="s">
-        <v>143</v>
+        <v>136</v>
       </c>
       <c r="B198">
         <v>1</v>
       </c>
       <c r="C198" t="s">
-        <v>259</v>
+        <v>137</v>
       </c>
       <c r="D198" t="s">
         <v>230</v>
@@ -3951,7 +4034,7 @@
     </row>
     <row r="199" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A199" t="s">
-        <v>144</v>
+        <v>143</v>
       </c>
       <c r="B199">
         <v>1</v>
@@ -3965,13 +4048,13 @@
     </row>
     <row r="200" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A200" t="s">
-        <v>149</v>
+        <v>144</v>
       </c>
       <c r="B200">
         <v>1</v>
       </c>
       <c r="C200" t="s">
-        <v>249</v>
+        <v>259</v>
       </c>
       <c r="D200" t="s">
         <v>230</v>
@@ -3979,7 +4062,7 @@
     </row>
     <row r="201" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A201" t="s">
-        <v>150</v>
+        <v>149</v>
       </c>
       <c r="B201">
         <v>1</v>
@@ -3993,49 +4076,49 @@
     </row>
     <row r="202" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A202" t="s">
-        <v>152</v>
+        <v>150</v>
       </c>
       <c r="B202">
         <v>1</v>
       </c>
       <c r="C202" t="s">
-        <v>155</v>
+        <v>249</v>
       </c>
       <c r="D202" t="s">
-        <v>264</v>
+        <v>230</v>
       </c>
     </row>
     <row r="203" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A203" t="s">
-        <v>156</v>
+        <v>152</v>
       </c>
       <c r="B203">
         <v>1</v>
       </c>
       <c r="C203" t="s">
-        <v>232</v>
+        <v>155</v>
       </c>
       <c r="D203" t="s">
-        <v>230</v>
+        <v>264</v>
       </c>
     </row>
     <row r="204" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A204" t="s">
-        <v>159</v>
+        <v>156</v>
       </c>
       <c r="B204">
         <v>1</v>
       </c>
       <c r="C204" t="s">
-        <v>260</v>
+        <v>232</v>
       </c>
       <c r="D204" t="s">
-        <v>263</v>
+        <v>230</v>
       </c>
     </row>
     <row r="205" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A205" t="s">
-        <v>160</v>
+        <v>159</v>
       </c>
       <c r="B205">
         <v>1</v>
@@ -4049,49 +4132,49 @@
     </row>
     <row r="206" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A206" t="s">
-        <v>164</v>
+        <v>160</v>
       </c>
       <c r="B206">
         <v>1</v>
       </c>
       <c r="C206" t="s">
-        <v>164</v>
+        <v>260</v>
       </c>
       <c r="D206" t="s">
-        <v>262</v>
+        <v>263</v>
       </c>
     </row>
     <row r="207" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A207" t="s">
-        <v>172</v>
+        <v>164</v>
       </c>
       <c r="B207">
         <v>1</v>
       </c>
       <c r="C207" t="s">
-        <v>222</v>
+        <v>164</v>
       </c>
       <c r="D207" t="s">
-        <v>230</v>
+        <v>262</v>
       </c>
     </row>
     <row r="208" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A208" t="s">
-        <v>174</v>
+        <v>172</v>
       </c>
       <c r="B208">
         <v>1</v>
       </c>
       <c r="C208" t="s">
-        <v>155</v>
+        <v>222</v>
       </c>
       <c r="D208" t="s">
-        <v>264</v>
+        <v>230</v>
       </c>
     </row>
     <row r="209" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A209" t="s">
-        <v>179</v>
+        <v>174</v>
       </c>
       <c r="B209">
         <v>1</v>
@@ -4105,7 +4188,7 @@
     </row>
     <row r="210" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A210" t="s">
-        <v>182</v>
+        <v>179</v>
       </c>
       <c r="B210">
         <v>1</v>
@@ -4119,7 +4202,7 @@
     </row>
     <row r="211" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A211" t="s">
-        <v>184</v>
+        <v>182</v>
       </c>
       <c r="B211">
         <v>1</v>
@@ -4133,7 +4216,7 @@
     </row>
     <row r="212" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A212" t="s">
-        <v>185</v>
+        <v>184</v>
       </c>
       <c r="B212">
         <v>1</v>
@@ -4147,13 +4230,13 @@
     </row>
     <row r="213" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A213" t="s">
-        <v>187</v>
+        <v>185</v>
       </c>
       <c r="B213">
         <v>1</v>
       </c>
       <c r="C213" t="s">
-        <v>181</v>
+        <v>155</v>
       </c>
       <c r="D213" t="s">
         <v>264</v>
@@ -4161,13 +4244,13 @@
     </row>
     <row r="214" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A214" t="s">
-        <v>188</v>
+        <v>187</v>
       </c>
       <c r="B214">
         <v>1</v>
       </c>
       <c r="C214" t="s">
-        <v>255</v>
+        <v>181</v>
       </c>
       <c r="D214" t="s">
         <v>264</v>
@@ -4175,13 +4258,13 @@
     </row>
     <row r="215" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A215" t="s">
-        <v>196</v>
+        <v>188</v>
       </c>
       <c r="B215">
         <v>1</v>
       </c>
       <c r="C215" t="s">
-        <v>258</v>
+        <v>255</v>
       </c>
       <c r="D215" t="s">
         <v>264</v>
@@ -4189,41 +4272,41 @@
     </row>
     <row r="216" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A216" t="s">
-        <v>198</v>
+        <v>196</v>
       </c>
       <c r="B216">
         <v>1</v>
       </c>
       <c r="C216" t="s">
-        <v>199</v>
+        <v>258</v>
       </c>
       <c r="D216" t="s">
-        <v>229</v>
+        <v>264</v>
       </c>
     </row>
     <row r="217" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A217" t="s">
-        <v>202</v>
+        <v>198</v>
       </c>
       <c r="B217">
         <v>1</v>
       </c>
       <c r="C217" t="s">
-        <v>173</v>
+        <v>199</v>
       </c>
       <c r="D217" t="s">
-        <v>262</v>
+        <v>229</v>
       </c>
     </row>
     <row r="218" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A218" t="s">
-        <v>203</v>
+        <v>202</v>
       </c>
       <c r="B218">
         <v>1</v>
       </c>
       <c r="C218" t="s">
-        <v>250</v>
+        <v>173</v>
       </c>
       <c r="D218" t="s">
         <v>262</v>
@@ -4231,41 +4314,41 @@
     </row>
     <row r="219" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A219" t="s">
-        <v>208</v>
+        <v>203</v>
       </c>
       <c r="B219">
         <v>1</v>
       </c>
       <c r="C219" t="s">
-        <v>231</v>
+        <v>250</v>
       </c>
       <c r="D219" t="s">
-        <v>229</v>
+        <v>262</v>
       </c>
     </row>
     <row r="220" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A220" t="s">
-        <v>213</v>
+        <v>208</v>
       </c>
       <c r="B220">
         <v>1</v>
       </c>
       <c r="C220" t="s">
-        <v>250</v>
+        <v>231</v>
       </c>
       <c r="D220" t="s">
-        <v>262</v>
+        <v>229</v>
       </c>
     </row>
     <row r="221" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A221" t="s">
-        <v>218</v>
+        <v>213</v>
       </c>
       <c r="B221">
         <v>1</v>
       </c>
       <c r="C221" t="s">
-        <v>173</v>
+        <v>250</v>
       </c>
       <c r="D221" t="s">
         <v>262</v>
@@ -4273,16 +4356,257 @@
     </row>
     <row r="222" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A222" t="s">
+        <v>218</v>
+      </c>
+      <c r="B222">
+        <v>1</v>
+      </c>
+      <c r="C222" t="s">
+        <v>173</v>
+      </c>
+      <c r="D222" t="s">
+        <v>262</v>
+      </c>
+    </row>
+    <row r="223" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A223" t="s">
         <v>261</v>
       </c>
-      <c r="B222">
-        <v>1</v>
-      </c>
-      <c r="C222" t="s">
+      <c r="B223">
+        <v>1</v>
+      </c>
+      <c r="C223" t="s">
         <v>232</v>
       </c>
-      <c r="D222" t="s">
-        <v>230</v>
+      <c r="D223" t="s">
+        <v>230</v>
+      </c>
+    </row>
+    <row r="224" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A224" t="s">
+        <v>265</v>
+      </c>
+      <c r="B224">
+        <v>1</v>
+      </c>
+      <c r="C224" t="s">
+        <v>252</v>
+      </c>
+      <c r="D224" t="s">
+        <v>263</v>
+      </c>
+    </row>
+    <row r="225" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A225" t="s">
+        <v>266</v>
+      </c>
+      <c r="B225">
+        <v>2</v>
+      </c>
+      <c r="C225" t="s">
+        <v>266</v>
+      </c>
+      <c r="D225" t="s">
+        <v>264</v>
+      </c>
+    </row>
+    <row r="226" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A226" t="s">
+        <v>267</v>
+      </c>
+      <c r="C226" t="s">
+        <v>232</v>
+      </c>
+      <c r="D226" t="s">
+        <v>230</v>
+      </c>
+    </row>
+    <row r="227" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A227" t="s">
+        <v>268</v>
+      </c>
+      <c r="C227" t="s">
+        <v>225</v>
+      </c>
+      <c r="D227" t="s">
+        <v>227</v>
+      </c>
+    </row>
+    <row r="228" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A228" t="s">
+        <v>269</v>
+      </c>
+      <c r="C228" t="s">
+        <v>225</v>
+      </c>
+      <c r="D228" t="s">
+        <v>227</v>
+      </c>
+    </row>
+    <row r="229" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A229" t="s">
+        <v>270</v>
+      </c>
+      <c r="C229" t="s">
+        <v>35</v>
+      </c>
+      <c r="D229" t="s">
+        <v>234</v>
+      </c>
+    </row>
+    <row r="230" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A230" t="s">
+        <v>271</v>
+      </c>
+      <c r="C230" t="s">
+        <v>225</v>
+      </c>
+      <c r="D230" t="s">
+        <v>227</v>
+      </c>
+    </row>
+    <row r="231" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A231" t="s">
+        <v>272</v>
+      </c>
+      <c r="B231">
+        <v>2</v>
+      </c>
+      <c r="C231" t="s">
+        <v>240</v>
+      </c>
+      <c r="D231" t="s">
+        <v>228</v>
+      </c>
+    </row>
+    <row r="232" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A232" t="s">
+        <v>274</v>
+      </c>
+      <c r="B232">
+        <v>5</v>
+      </c>
+      <c r="C232" t="s">
+        <v>273</v>
+      </c>
+      <c r="D232" t="s">
+        <v>228</v>
+      </c>
+    </row>
+    <row r="233" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A233" t="s">
+        <v>275</v>
+      </c>
+      <c r="B233">
+        <v>4</v>
+      </c>
+      <c r="C233" t="s">
+        <v>275</v>
+      </c>
+      <c r="D233" t="s">
+        <v>228</v>
+      </c>
+    </row>
+    <row r="234" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A234" t="s">
+        <v>222</v>
+      </c>
+      <c r="C234" t="s">
+        <v>222</v>
+      </c>
+      <c r="D234" t="s">
+        <v>230</v>
+      </c>
+    </row>
+    <row r="235" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A235" t="s">
+        <v>276</v>
+      </c>
+      <c r="C235" t="s">
+        <v>70</v>
+      </c>
+      <c r="D235" t="s">
+        <v>230</v>
+      </c>
+    </row>
+    <row r="236" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A236" t="s">
+        <v>277</v>
+      </c>
+      <c r="C236" t="s">
+        <v>140</v>
+      </c>
+      <c r="D236" t="s">
+        <v>230</v>
+      </c>
+    </row>
+    <row r="237" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A237" t="s">
+        <v>278</v>
+      </c>
+      <c r="B237">
+        <v>1</v>
+      </c>
+      <c r="C237" t="s">
+        <v>240</v>
+      </c>
+      <c r="D237" t="s">
+        <v>228</v>
+      </c>
+    </row>
+    <row r="238" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A238" t="s">
+        <v>279</v>
+      </c>
+      <c r="C238" t="s">
+        <v>140</v>
+      </c>
+      <c r="D238" t="s">
+        <v>230</v>
+      </c>
+    </row>
+    <row r="239" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A239" t="s">
+        <v>281</v>
+      </c>
+      <c r="C239" t="s">
+        <v>280</v>
+      </c>
+      <c r="D239" t="s">
+        <v>237</v>
+      </c>
+    </row>
+    <row r="240" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A240" t="s">
+        <v>282</v>
+      </c>
+      <c r="C240" t="s">
+        <v>283</v>
+      </c>
+      <c r="D240" t="s">
+        <v>264</v>
+      </c>
+    </row>
+    <row r="241" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A241" t="s">
+        <v>286</v>
+      </c>
+      <c r="C241" t="s">
+        <v>240</v>
+      </c>
+      <c r="D241" t="s">
+        <v>228</v>
+      </c>
+    </row>
+    <row r="242" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A242" t="s">
+        <v>285</v>
+      </c>
+      <c r="C242" t="s">
+        <v>285</v>
+      </c>
+      <c r="D242" t="s">
+        <v>262</v>
       </c>
     </row>
   </sheetData>

</xml_diff>